<commit_message>
added all named authors
</commit_message>
<xml_diff>
--- a/Authors to be added.xlsx
+++ b/Authors to be added.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D1A726-8461-49EC-A58D-ABB05D48444E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86874C6F-542F-4D97-A9C0-766F57153174}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>http://viaf.org/viaf/287131971</t>
+  </si>
+  <si>
+    <t>Saleius Bassus</t>
+  </si>
+  <si>
+    <t>entry 3156</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/255045890</t>
+  </si>
+  <si>
+    <t>entry 3838</t>
   </si>
 </sst>
 </file>
@@ -411,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,6 +506,28 @@
         <v>17</v>
       </c>
     </row>
+    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{CDF89061-4F05-4F6D-9E96-2C39F6E0EFB5}"/>

</xml_diff>

<commit_message>
worked on engelmann AK and engelmann RR copy
</commit_message>
<xml_diff>
--- a/Authors to be added.xlsx
+++ b/Authors to be added.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86874C6F-542F-4D97-A9C0-766F57153174}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1DAE2A-1B57-4C43-BFCA-0D8FC4566899}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>entry 3838</t>
+  </si>
+  <si>
+    <t>Hostius</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,6 +531,11 @@
         <v>21</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{CDF89061-4F05-4F6D-9E96-2C39F6E0EFB5}"/>

</xml_diff>

<commit_message>
same old same old
</commit_message>
<xml_diff>
--- a/Authors to be added.xlsx
+++ b/Authors to be added.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8104EC0B-7DFC-4925-9032-2C50A486B032}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3808877E-3028-4783-B72F-322DC80DA916}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>pierre de corbeil</t>
+  </si>
+  <si>
+    <t>Atilius Fortunatianus</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -544,6 +547,11 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{CDF89061-4F05-4F6D-9E96-2C39F6E0EFB5}"/>

</xml_diff>

<commit_message>
consolodated Wernsdorf's poetae minores, etc.
</commit_message>
<xml_diff>
--- a/Authors to be added.xlsx
+++ b/Authors to be added.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3808877E-3028-4783-B72F-322DC80DA916}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB045B6E-7BCB-48BA-B63C-C91931E2D76F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>Atilius Fortunatianus</t>
+  </si>
+  <si>
+    <t>Vomanus?</t>
+  </si>
+  <si>
+    <t>Ofilius?</t>
+  </si>
+  <si>
+    <t>Speratus?</t>
   </si>
 </sst>
 </file>
@@ -432,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -552,6 +561,21 @@
         <v>24</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{CDF89061-4F05-4F6D-9E96-2C39F6E0EFB5}"/>

</xml_diff>

<commit_message>
more off the same
</commit_message>
<xml_diff>
--- a/Authors to be added.xlsx
+++ b/Authors to be added.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB045B6E-7BCB-48BA-B63C-C91931E2D76F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3E50DC-654E-43E5-8AA9-981A41757786}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -104,6 +104,21 @@
   </si>
   <si>
     <t>Speratus?</t>
+  </si>
+  <si>
+    <t>eucharia</t>
+  </si>
+  <si>
+    <t>Aemelius Magnus Arborius</t>
+  </si>
+  <si>
+    <t>Lamaire PLM v2</t>
+  </si>
+  <si>
+    <t>Gaius Cassius Parmensis</t>
+  </si>
+  <si>
+    <t>Lemaire PLM v</t>
   </si>
 </sst>
 </file>
@@ -441,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -576,6 +591,30 @@
         <v>27</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{CDF89061-4F05-4F6D-9E96-2C39F6E0EFB5}"/>

</xml_diff>